<commit_message>
fini le plan de test
</commit_message>
<xml_diff>
--- a/Plan de Test.xlsx
+++ b/Plan de Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\JWDP5\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74024331-ED18-42A7-8764-0EBCB019098E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B85184-8E4F-49BB-946C-E6AFB0E6D63D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8B526EB1-2F09-4841-9884-4E1F77679833}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -63,24 +63,15 @@
     <t>fetchUse</t>
   </si>
   <si>
-    <t>Observer la valeur retournée dans la console Google Chrome avec un console,log par exemple, Ou changer une partie de l'URL(ce qui ne donnera pas de résultat)</t>
-  </si>
-  <si>
     <t>La fonction doit effectuer une promise vers l'URL donnée (API)</t>
   </si>
   <si>
-    <t>Si la fonction/URL est mal décrite, alors il n'y aura pas de promise vers l'API</t>
-  </si>
-  <si>
     <t>Ligne 6 a 36</t>
   </si>
   <si>
     <t>template</t>
   </si>
   <si>
-    <t>La Fonction doit récuperer les données de l'API et les traduire en format Javascript pour pouvoir me servir de ces données, ensuite, elle sélectionne l'endroit ou afficher mes données sur ma page web, puis elle clone mes "blocks" d'affichage autant de fois qu'il y a d'élements different,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ma page web n'affiche pas les éléments, ou s'il ne sont pas au bon endroit, si le clonage de mes blocks ne se font pas.</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>La Fonction récupère les données de l'id qui à été sellectionné et affiche les données au bon endroit sur ma page web. Elle ajoute aussi un style de couleurs pour chaques colors de mon article.</t>
   </si>
   <si>
-    <t>L'id de l'article n'est pas récupérer si la fonction n'est pas bien paramétrer, la promise n'est pas résolu ou l'URL n'est pas correcte.</t>
-  </si>
-  <si>
     <t>Vérifier que mon articles s'affiche correctement sur ma page, que mes styles de couleurs se mette en forme, que mes données soit affiché au bon endroit, observer que la valeur retournée dans la console Google Chrome avec un console.log corresponde bien aux informations de l'id qui à été sélèctionné.</t>
   </si>
   <si>
@@ -148,6 +136,36 @@
   </si>
   <si>
     <t>Mauvaise ecriture de code qui entrainerai un message d'erreur, qui ne declencherai pas ma fonction ou qui ne recupererai pas l'article en question</t>
+  </si>
+  <si>
+    <t>Panier.js</t>
+  </si>
+  <si>
+    <t>Ligne 50 à 94</t>
+  </si>
+  <si>
+    <t>onClickButton(e)</t>
+  </si>
+  <si>
+    <t>Fonction qui place les .values du formulaire dans un Objet, qui place aussi les _id de chaques articles sélèctionné dans un tableau, et qui au final place l'objet valeur + le [_id] dans un objet afin de l'envoyé vers le serveur en méthode POST. La fonction crée/stock aussi une valeur orderId dans le localStorage.</t>
+  </si>
+  <si>
+    <t>On peut verifier le resultat grace au console.log pour voir si l'objet/tableau ont bien été crée, si orderId à bien été stocker dans le localStorage, Si la methode POST de l'envoi au serveur c'est bien effectué et quon a bien en retour le numéros de commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que les values formulaire soit mal récuperer, que l'objet et le tableau soit mal défini ou que la méthode POST soit mal appelée ce qui refait une requete au serveur non valide </t>
+  </si>
+  <si>
+    <t>Observer la valeur retournée dans la console Google Chrome avec un console.log par exemple, Ou changer une partie de l'URL(ce qui ne donnera pas de résultat).</t>
+  </si>
+  <si>
+    <t>Si la fonction/URL est mal décrite, alors il n'y aura pas de promise vers l'API.</t>
+  </si>
+  <si>
+    <t>La Fonction doit récuperer les données de l'API et les traduire en format Javascript pour pouvoir me servir de ces données, ensuite, elle sélectionne l'endroit ou afficher mes données sur ma page web, puis elle clone mes "blocks" d'affichage autant de fois qu'il y a d'élements differents.</t>
+  </si>
+  <si>
+    <t>L'id de l'article n'est pas récupéré si la fonction n'est pas bien paramétré, la promise n'est pas résolu ou l'URL n'est pas correcte.</t>
   </si>
 </sst>
 </file>
@@ -163,15 +181,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,31 +230,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,16 +245,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -557,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC8C431-D8B6-4A23-A381-9C220601DE34}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,33 +626,33 @@
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -642,83 +664,83 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>25</v>
+      <c r="G6" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="G7" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,13 +751,25 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+    <row r="11" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -801,14 +835,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
+    <row r="20" spans="2:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>

</xml_diff>

<commit_message>
Projet Fini, reste a préparer soutenance
</commit_message>
<xml_diff>
--- a/Plan de Test.xlsx
+++ b/Plan de Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Git\JWDP5\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7B9301-A4F4-47FE-B153-D9543AB10EF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4251D24-AE97-47ED-A6F8-0A8682B35DA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8B526EB1-2F09-4841-9884-4E1F77679833}"/>
   </bookViews>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC8C431-D8B6-4A23-A381-9C220601DE34}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,13 +925,13 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="5">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F17" s="5">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G17" s="13">
-        <v>0.89470000000000005</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>